<commit_message>
fix page insert problem by change sql column status in db fix input form select name with quote
</commit_message>
<xml_diff>
--- a/rsc/neoserver_page_info.xlsx
+++ b/rsc/neoserver_page_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app\neo_server\rsc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FCC506-C728-43FF-9BC6-3FB15AF270DB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3E6A0A-4AB9-4648-B718-73B07B4D580D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="4728" xr2:uid="{B0E0DE65-FA25-4D03-8955-531C0911F340}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>webtoon</t>
   </si>
@@ -390,6 +390,14 @@
    seq  ,tdc_uid  ,title  ,issue  ,solution ,status   ,updt_date  ,reg_date
 ) VALUES (
     {last_seq}  ,'{last_uid}'   ,'{title}'  ,'{issue}'   ,'{solution}'  ,''  ,now()  ,now() 
+)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INSERT INTO neo_pwinfo.webtoon(
+   seq  ,wtn_uid  ,prt_uid  ,title   ,id  ,dates ,status    ,updt_date  ,reg_date 
+) VALUES (
+   {last_seq}  ,'{last_uid}'  ,'{prt_uid}'  ,'{title}'   ,'{id}'  ,'{dates}'  ,'',now()  ,now()
 )</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -761,10 +769,10 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" outlineLevelCol="1" x14ac:dyDescent="0.4"/>
@@ -856,7 +864,7 @@
         <v>45</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
update dynamic function for lay out col input
</commit_message>
<xml_diff>
--- a/rsc/neoserver_page_info.xlsx
+++ b/rsc/neoserver_page_info.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app\neo_server\rsc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\PYSERVER\src\neo_server\rsc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52B2299-C5C1-4F1F-822E-4EF573C2099F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -461,7 +460,7 @@
   <si>
     <t xml:space="preserve">SELECT seq, hlt_uid as cur_uid, sys_bp, dia_bp, pulse, weight, param, type, updt_date, reg_date, comment, 
 CONCAT(sys_bp,'/' ,dia_bp,'(', pulse,')') as bp,
-DATE_FORMAT(reg_date, "%m/%d %H:%i") as dt,
+DATE_FORMAT(reg_date, "%Y-%m-%d %H:%i:%S") as dt,
 SUBSTR( _UTF8'일월화수목금토', DAYOFWEEK(reg_date), 1) AS week
 FROM health where True {extra_condition} order by reg_date desc
 </t>
@@ -471,7 +470,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -831,7 +830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -841,23 +840,23 @@
       <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" outlineLevelCol="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.19921875" customWidth="1"/>
-    <col min="3" max="3" width="25.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.8984375" customWidth="1"/>
-    <col min="5" max="5" width="20.09765625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.09765625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="42.59765625" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="19.19921875" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="30.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.25" customWidth="1"/>
+    <col min="3" max="3" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.875" customWidth="1"/>
+    <col min="5" max="5" width="20.125" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.125" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="42.625" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="19.25" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="30.875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.09765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -898,7 +897,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="174" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="165" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -933,7 +932,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -959,7 +958,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="243.6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" ht="231" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -997,7 +996,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="174" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" ht="165" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1038,7 +1037,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="121.8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1073,7 +1072,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="174" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" ht="198" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1116,19 +1115,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="12" width="27.19921875" customWidth="1"/>
+    <col min="10" max="12" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="191.4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1173,71 +1172,71 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1250,16 +1249,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
update show by login or logout
</commit_message>
<xml_diff>
--- a/rsc/neoserver_page_info.xlsx
+++ b/rsc/neoserver_page_info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\PYSERVER\src\neo_server\rsc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app\neo_server\rsc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB38F382-EC4C-44B1-919F-DB4D51B0E07A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="91">
   <si>
     <t>webtoon</t>
   </si>
@@ -466,11 +467,15 @@
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>general</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -830,33 +835,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" outlineLevelCol="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.25" customWidth="1"/>
-    <col min="3" max="3" width="25.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.875" customWidth="1"/>
-    <col min="5" max="5" width="20.125" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.125" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="42.625" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="19.25" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="30.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.19921875" customWidth="1"/>
+    <col min="3" max="3" width="25.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.8984375" customWidth="1"/>
+    <col min="5" max="5" width="20.09765625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.09765625" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="42.59765625" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="19.19921875" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="30.8984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -897,7 +902,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="165" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="174" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -931,8 +936,11 @@
       <c r="L2" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M2" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -957,8 +965,11 @@
       <c r="I3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="231" x14ac:dyDescent="0.3">
+      <c r="M3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="243.6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -995,8 +1006,11 @@
       <c r="L4" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="165" x14ac:dyDescent="0.3">
+      <c r="M4" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="174" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1037,7 +1051,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="121.8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1071,8 +1085,11 @@
       <c r="L6" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="198" x14ac:dyDescent="0.3">
+      <c r="M6" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="174" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1105,6 +1122,9 @@
       </c>
       <c r="L7" s="1" t="s">
         <v>76</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1115,19 +1135,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="10" max="12" width="27.25" customWidth="1"/>
+    <col min="10" max="12" width="27.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="191.4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1172,71 +1192,71 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1249,16 +1269,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1296,7 +1316,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>13</v>
       </c>

</xml_diff>